<commit_message>
Update program with reference to supplier's name
</commit_message>
<xml_diff>
--- a/Excel sheets/Root Causes.xlsx
+++ b/Excel sheets/Root Causes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a12a3dfde7402925/Documentos/Programming/Python/Root Cause Analysis/Excel sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC10489C01D97B405ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E75B24EC-8F16-473E-9F04-472D7450B64E}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_F25DC773A252ABDACC10489C01D97B405ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EF4B7D5-ABB6-4A46-A825-31B996B5261B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10690" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="10580" windowWidth="19310" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Machine</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>Repair</t>
+  </si>
+  <si>
+    <t>Internal control</t>
+  </si>
+  <si>
+    <t>Not clear instruction</t>
+  </si>
+  <si>
+    <t>Drawing update</t>
   </si>
 </sst>
 </file>
@@ -101,10 +110,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,6 +426,21 @@
         <v>7</v>
       </c>
     </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>